<commit_message>
correct bond price and county data length
</commit_message>
<xml_diff>
--- a/Final Data/Ohio/1 ohio counties dataset from pandas.xlsx
+++ b/Final Data/Ohio/1 ohio counties dataset from pandas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CL273"/>
+  <dimension ref="A1:CL272"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -69060,280 +69060,6 @@
         <v>116951</v>
       </c>
     </row>
-    <row r="273">
-      <c r="A273" s="1" t="n">
-        <v>271</v>
-      </c>
-      <c r="B273" t="inlineStr">
-        <is>
-          <t>2022-08-31</t>
-        </is>
-      </c>
-      <c r="C273" t="n">
-        <v>286187</v>
-      </c>
-      <c r="D273" t="n">
-        <v>199777</v>
-      </c>
-      <c r="E273" t="n">
-        <v>239838</v>
-      </c>
-      <c r="F273" t="n">
-        <v>200731</v>
-      </c>
-      <c r="G273" t="n">
-        <v>169385</v>
-      </c>
-      <c r="H273" t="n">
-        <v>151522</v>
-      </c>
-      <c r="I273" t="n">
-        <v>272080</v>
-      </c>
-      <c r="J273" t="n">
-        <v>187070</v>
-      </c>
-      <c r="K273" t="n">
-        <v>219631</v>
-      </c>
-      <c r="L273" t="n">
-        <v>149700</v>
-      </c>
-      <c r="M273" t="n">
-        <v>215052</v>
-      </c>
-      <c r="N273" t="n">
-        <v>348978</v>
-      </c>
-      <c r="O273" t="n">
-        <v>278917</v>
-      </c>
-      <c r="P273" t="n">
-        <v>468091</v>
-      </c>
-      <c r="Q273" t="n">
-        <v>146466</v>
-      </c>
-      <c r="R273" t="n">
-        <v>309102</v>
-      </c>
-      <c r="S273" t="n">
-        <v>300085</v>
-      </c>
-      <c r="T273" t="n">
-        <v>255594</v>
-      </c>
-      <c r="U273" t="n">
-        <v>236082</v>
-      </c>
-      <c r="V273" t="n">
-        <v>322719</v>
-      </c>
-      <c r="W273" t="n">
-        <v>166023</v>
-      </c>
-      <c r="X273" t="n">
-        <v>232989</v>
-      </c>
-      <c r="Y273" t="n">
-        <v>170391</v>
-      </c>
-      <c r="Z273" t="n">
-        <v>415655</v>
-      </c>
-      <c r="AA273" t="n">
-        <v>221148</v>
-      </c>
-      <c r="AB273" t="n">
-        <v>136489</v>
-      </c>
-      <c r="AC273" t="n">
-        <v>166082</v>
-      </c>
-      <c r="AD273" t="n">
-        <v>154469</v>
-      </c>
-      <c r="AE273" t="n">
-        <v>320936</v>
-      </c>
-      <c r="AF273" t="n">
-        <v>178152</v>
-      </c>
-      <c r="AG273" t="n">
-        <v>173397</v>
-      </c>
-      <c r="AH273" t="n">
-        <v>168535</v>
-      </c>
-      <c r="AI273" t="n">
-        <v>108738</v>
-      </c>
-      <c r="AJ273" t="n">
-        <v>205563</v>
-      </c>
-      <c r="AK273" t="n">
-        <v>204581</v>
-      </c>
-      <c r="AL273" t="n">
-        <v>140404</v>
-      </c>
-      <c r="AM273" t="n">
-        <v>111206</v>
-      </c>
-      <c r="AN273" t="n">
-        <v>174310</v>
-      </c>
-      <c r="AO273" t="n">
-        <v>136833</v>
-      </c>
-      <c r="AP273" t="n">
-        <v>214427</v>
-      </c>
-      <c r="AQ273" t="n">
-        <v>134357</v>
-      </c>
-      <c r="AR273" t="n">
-        <v>171140</v>
-      </c>
-      <c r="AS273" t="n">
-        <v>156349</v>
-      </c>
-      <c r="AT273" t="n">
-        <v>158747</v>
-      </c>
-      <c r="AU273" t="n">
-        <v>244495</v>
-      </c>
-      <c r="AV273" t="n">
-        <v>363999</v>
-      </c>
-      <c r="AW273" t="n">
-        <v>144434</v>
-      </c>
-      <c r="AX273" t="n">
-        <v>185908</v>
-      </c>
-      <c r="AY273" t="n">
-        <v>178648</v>
-      </c>
-      <c r="AZ273" t="n">
-        <v>203301</v>
-      </c>
-      <c r="BA273" t="n">
-        <v>197126</v>
-      </c>
-      <c r="BB273" t="n">
-        <v>191544</v>
-      </c>
-      <c r="BC273" t="n">
-        <v>251258</v>
-      </c>
-      <c r="BD273" t="n">
-        <v>280099</v>
-      </c>
-      <c r="BE273" t="n">
-        <v>187200</v>
-      </c>
-      <c r="BF273" t="n">
-        <v>150129</v>
-      </c>
-      <c r="BG273" t="n">
-        <v>193017</v>
-      </c>
-      <c r="BH273" t="n">
-        <v>187405</v>
-      </c>
-      <c r="BI273" t="n">
-        <v>114678</v>
-      </c>
-      <c r="BJ273" t="n">
-        <v>182539</v>
-      </c>
-      <c r="BK273" t="n">
-        <v>214091</v>
-      </c>
-      <c r="BL273" t="n">
-        <v>228459</v>
-      </c>
-      <c r="BM273" t="n">
-        <v>138125</v>
-      </c>
-      <c r="BN273" t="n">
-        <v>189735</v>
-      </c>
-      <c r="BO273" t="n">
-        <v>160737</v>
-      </c>
-      <c r="BP273" t="n">
-        <v>146718</v>
-      </c>
-      <c r="BQ273" t="n">
-        <v>151488</v>
-      </c>
-      <c r="BR273" t="n">
-        <v>165139</v>
-      </c>
-      <c r="BS273" t="n">
-        <v>220410</v>
-      </c>
-      <c r="BT273" t="n">
-        <v>196698</v>
-      </c>
-      <c r="BU273" t="n">
-        <v>112227</v>
-      </c>
-      <c r="BV273" t="n">
-        <v>146344</v>
-      </c>
-      <c r="BW273" t="n">
-        <v>140212</v>
-      </c>
-      <c r="BX273" t="n">
-        <v>160851</v>
-      </c>
-      <c r="BY273" t="n">
-        <v>183602</v>
-      </c>
-      <c r="BZ273" t="n">
-        <v>135610</v>
-      </c>
-      <c r="CA273" t="n">
-        <v>145409</v>
-      </c>
-      <c r="CB273" t="n">
-        <v>135914</v>
-      </c>
-      <c r="CC273" t="n">
-        <v>178705</v>
-      </c>
-      <c r="CD273" t="n">
-        <v>171066</v>
-      </c>
-      <c r="CE273" t="n">
-        <v>107721</v>
-      </c>
-      <c r="CF273" t="n">
-        <v>158194</v>
-      </c>
-      <c r="CG273" t="n">
-        <v>124238</v>
-      </c>
-      <c r="CH273" t="n">
-        <v>120956</v>
-      </c>
-      <c r="CI273" t="n">
-        <v>134919</v>
-      </c>
-      <c r="CJ273" t="n">
-        <v>175469</v>
-      </c>
-      <c r="CK273" t="n">
-        <v>134839</v>
-      </c>
-      <c r="CL273" t="n">
-        <v>118336</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>